<commit_message>
Stückliste aktualisiert (Akku, Motor, Schleifring)
</commit_message>
<xml_diff>
--- a/Hardware/Stückliste.xlsx
+++ b/Hardware/Stückliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgaer\Google Drive\Fachhochschule\4.Semester\pro4E\gitHub\pro4e\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3762A8D5-26CA-4B15-B084-A3B9692515E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6C0830-7B43-4115-9279-1CFBA042016F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>Position</t>
   </si>
@@ -191,6 +191,45 @@
   </si>
   <si>
     <t>732-1151-1-ND</t>
+  </si>
+  <si>
+    <t>Getriebemotor 12 V</t>
+  </si>
+  <si>
+    <t>Conrad</t>
+  </si>
+  <si>
+    <t>IG320005-3AC21R</t>
+  </si>
+  <si>
+    <t>234253 - UP</t>
+  </si>
+  <si>
+    <t>4S LiPo Akku 500mAh</t>
+  </si>
+  <si>
+    <t>Hobbyking</t>
+  </si>
+  <si>
+    <t>9067000341-0</t>
+  </si>
+  <si>
+    <t>4mm Gold-Steckverbinder 10 Stk.</t>
+  </si>
+  <si>
+    <t>servo technica</t>
+  </si>
+  <si>
+    <t>SVTS C 03-X-A-00/06</t>
+  </si>
+  <si>
+    <t>Schleifring</t>
+  </si>
+  <si>
+    <t>DL-Volt-Alarm</t>
+  </si>
+  <si>
+    <t>Lipoly Niederspannungs-Warnung (2s ~ 4s)</t>
   </si>
 </sst>
 </file>
@@ -559,14 +598,14 @@
   <dimension ref="B2:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.84375" customWidth="1"/>
     <col min="2" max="2" width="10.3828125" customWidth="1"/>
-    <col min="3" max="3" width="20.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.4609375" customWidth="1"/>
     <col min="4" max="4" width="21.15234375" customWidth="1"/>
     <col min="5" max="5" width="15.15234375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.84375" bestFit="1" customWidth="1"/>
@@ -878,46 +917,132 @@
       <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>27.95</v>
+      </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27.95</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>30.12</v>
+      </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30.12</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B14" s="1">
         <v>12</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="3">
+        <v>15000068</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3.16</v>
+      </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B15" s="1">
         <v>13</v>
       </c>
-      <c r="I15" s="2"/>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2.63</v>
+      </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B16" s="1">
         <v>14</v>
       </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
@@ -1090,7 +1215,7 @@
       </c>
       <c r="J34" s="2">
         <f>SUM(J3:J33)</f>
-        <v>131.48600000000002</v>
+        <v>195.346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Stückliste (dual opamp), pdf vom Schema, Feedback PH
</commit_message>
<xml_diff>
--- a/Hardware/Stückliste.xlsx
+++ b/Hardware/Stückliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenny\Documents\GitHub\pro4e\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\GitHub\pro4e\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80069CDB-D6A8-4AB2-8F9C-64C33A4606EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5DBF3A-B99C-40AF-A838-7B47DBE63AAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="450" windowWidth="19200" windowHeight="10010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="7920" windowWidth="21540" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -288,12 +288,6 @@
     <t>Verstärker</t>
   </si>
   <si>
-    <t>LMV796MF/NOPB</t>
-  </si>
-  <si>
-    <t>LMV796MF/NOPBCT-ND</t>
-  </si>
-  <si>
     <t>Quarzoszillator</t>
   </si>
   <si>
@@ -328,6 +322,12 @@
   </si>
   <si>
     <t>SER2207CT-ND</t>
+  </si>
+  <si>
+    <t>LMV797MM/NOPB</t>
+  </si>
+  <si>
+    <t>LMV797MM/NOPBCT-ND</t>
   </si>
 </sst>
 </file>
@@ -687,24 +687,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="36.453125" customWidth="1"/>
-    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -733,7 +733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -763,7 +763,7 @@
         <v>55.33</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -793,7 +793,7 @@
         <v>36.756</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -823,7 +823,7 @@
         <v>11.07</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -853,7 +853,7 @@
         <v>6.85</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -883,7 +883,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -913,7 +913,7 @@
         <v>27.95</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -940,7 +940,7 @@
         <v>30.12</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -967,7 +967,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -994,7 +994,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>0.94500000000000006</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>2.9699999999999998</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>29.38</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>21</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>23</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>24</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>25</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>26</v>
       </c>
@@ -1477,13 +1477,13 @@
         <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1492,28 +1492,28 @@
         <v>2</v>
       </c>
       <c r="I28" s="2">
-        <v>1.46</v>
+        <v>1.82</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" si="0"/>
-        <v>2.92</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>27</v>
       </c>
       <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
         <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" t="s">
-        <v>89</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1529,21 +1529,21 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G30">
         <v>2</v>
@@ -1559,21 +1559,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
         <v>93</v>
-      </c>
-      <c r="E31" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" t="s">
-        <v>95</v>
       </c>
       <c r="G31">
         <v>25</v>
@@ -1589,21 +1589,21 @@
         <v>1.7500000000000002</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>30</v>
       </c>
       <c r="C32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" t="s">
         <v>96</v>
-      </c>
-      <c r="D32" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" t="s">
-        <v>98</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1619,13 +1619,13 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="34" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
         <v>26</v>
       </c>
       <c r="J34" s="2">
         <f>SUM(J3:J33)</f>
-        <v>246.30099999999996</v>
+        <v>247.02099999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>